<commit_message>
effect features addded with some bugs it will be fixed in a few days
</commit_message>
<xml_diff>
--- a/cashflow.xlsx
+++ b/cashflow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eren\Desktop\Projects\discounted_cashflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eren\Desktop\Eren-Backup\Projects\discounted_cashflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC25C5A9-3AD1-46E6-A8B0-814DA8974F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB4557E-A3AC-4EEA-AFC2-490ACD14A33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="7">
   <si>
     <t>CF_Pattern</t>
   </si>
@@ -55,13 +55,16 @@
   <si>
     <t>uoa3</t>
   </si>
+  <si>
+    <t>uoa4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.0000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -106,7 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344448C0-5813-EF41-B935-311A4303076B}">
-  <dimension ref="A1:C541"/>
+  <dimension ref="A1:C721"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A522" workbookViewId="0">
-      <selection activeCell="B541" sqref="B541"/>
+    <sheetView tabSelected="1" topLeftCell="A664" workbookViewId="0">
+      <selection activeCell="E668" sqref="E668"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6347,6 +6350,1986 @@
         <v>-6.9963526754997698E-6</v>
       </c>
     </row>
+    <row r="542" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A542" t="s">
+        <v>6</v>
+      </c>
+      <c r="B542">
+        <v>1</v>
+      </c>
+      <c r="C542" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="543" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A543" t="s">
+        <v>6</v>
+      </c>
+      <c r="B543">
+        <v>2</v>
+      </c>
+      <c r="C543" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="544" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A544" t="s">
+        <v>6</v>
+      </c>
+      <c r="B544">
+        <v>3</v>
+      </c>
+      <c r="C544" s="1">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="545" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A545" t="s">
+        <v>6</v>
+      </c>
+      <c r="B545">
+        <v>4</v>
+      </c>
+      <c r="C545" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="546" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A546" t="s">
+        <v>6</v>
+      </c>
+      <c r="B546">
+        <v>5</v>
+      </c>
+      <c r="C546" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A547" t="s">
+        <v>6</v>
+      </c>
+      <c r="B547">
+        <v>6</v>
+      </c>
+      <c r="C547" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="548" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A548" t="s">
+        <v>6</v>
+      </c>
+      <c r="B548">
+        <v>7</v>
+      </c>
+      <c r="C548" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="549" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A549" t="s">
+        <v>6</v>
+      </c>
+      <c r="B549">
+        <v>8</v>
+      </c>
+      <c r="C549" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="550" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A550" t="s">
+        <v>6</v>
+      </c>
+      <c r="B550">
+        <v>9</v>
+      </c>
+      <c r="C550" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A551" t="s">
+        <v>6</v>
+      </c>
+      <c r="B551">
+        <v>10</v>
+      </c>
+      <c r="C551" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="552" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A552" t="s">
+        <v>6</v>
+      </c>
+      <c r="B552">
+        <v>11</v>
+      </c>
+      <c r="C552" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="553" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A553" t="s">
+        <v>6</v>
+      </c>
+      <c r="B553">
+        <v>12</v>
+      </c>
+      <c r="C553" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="554" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A554" t="s">
+        <v>6</v>
+      </c>
+      <c r="B554">
+        <v>13</v>
+      </c>
+      <c r="C554" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="555" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A555" t="s">
+        <v>6</v>
+      </c>
+      <c r="B555">
+        <v>14</v>
+      </c>
+      <c r="C555" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="556" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A556" t="s">
+        <v>6</v>
+      </c>
+      <c r="B556">
+        <v>15</v>
+      </c>
+      <c r="C556" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A557" t="s">
+        <v>6</v>
+      </c>
+      <c r="B557">
+        <v>16</v>
+      </c>
+      <c r="C557" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>6</v>
+      </c>
+      <c r="B558">
+        <v>17</v>
+      </c>
+      <c r="C558" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A559" t="s">
+        <v>6</v>
+      </c>
+      <c r="B559">
+        <v>18</v>
+      </c>
+      <c r="C559" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A560" t="s">
+        <v>6</v>
+      </c>
+      <c r="B560">
+        <v>19</v>
+      </c>
+      <c r="C560" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A561" t="s">
+        <v>6</v>
+      </c>
+      <c r="B561">
+        <v>20</v>
+      </c>
+      <c r="C561" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="562" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A562" t="s">
+        <v>6</v>
+      </c>
+      <c r="B562">
+        <v>21</v>
+      </c>
+      <c r="C562" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A563" t="s">
+        <v>6</v>
+      </c>
+      <c r="B563">
+        <v>22</v>
+      </c>
+      <c r="C563" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="564" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A564" t="s">
+        <v>6</v>
+      </c>
+      <c r="B564">
+        <v>23</v>
+      </c>
+      <c r="C564" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="565" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A565" t="s">
+        <v>6</v>
+      </c>
+      <c r="B565">
+        <v>24</v>
+      </c>
+      <c r="C565" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>6</v>
+      </c>
+      <c r="B566">
+        <v>25</v>
+      </c>
+      <c r="C566" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="567" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>6</v>
+      </c>
+      <c r="B567">
+        <v>26</v>
+      </c>
+      <c r="C567" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>6</v>
+      </c>
+      <c r="B568">
+        <v>27</v>
+      </c>
+      <c r="C568" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="569" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>6</v>
+      </c>
+      <c r="B569">
+        <v>28</v>
+      </c>
+      <c r="C569" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>6</v>
+      </c>
+      <c r="B570">
+        <v>29</v>
+      </c>
+      <c r="C570" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="571" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>6</v>
+      </c>
+      <c r="B571">
+        <v>30</v>
+      </c>
+      <c r="C571" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="572" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>6</v>
+      </c>
+      <c r="B572">
+        <v>31</v>
+      </c>
+      <c r="C572" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="573" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>6</v>
+      </c>
+      <c r="B573">
+        <v>32</v>
+      </c>
+      <c r="C573" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="574" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>6</v>
+      </c>
+      <c r="B574">
+        <v>33</v>
+      </c>
+      <c r="C574" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="575" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>6</v>
+      </c>
+      <c r="B575">
+        <v>34</v>
+      </c>
+      <c r="C575" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="576" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>6</v>
+      </c>
+      <c r="B576">
+        <v>35</v>
+      </c>
+      <c r="C576" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="577" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>6</v>
+      </c>
+      <c r="B577">
+        <v>36</v>
+      </c>
+      <c r="C577" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="578" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>6</v>
+      </c>
+      <c r="B578">
+        <v>37</v>
+      </c>
+      <c r="C578" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>6</v>
+      </c>
+      <c r="B579">
+        <v>38</v>
+      </c>
+      <c r="C579" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="580" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>6</v>
+      </c>
+      <c r="B580">
+        <v>39</v>
+      </c>
+      <c r="C580" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>6</v>
+      </c>
+      <c r="B581">
+        <v>40</v>
+      </c>
+      <c r="C581" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="582" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>6</v>
+      </c>
+      <c r="B582">
+        <v>41</v>
+      </c>
+      <c r="C582" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="583" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>6</v>
+      </c>
+      <c r="B583">
+        <v>42</v>
+      </c>
+      <c r="C583" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="584" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>6</v>
+      </c>
+      <c r="B584">
+        <v>43</v>
+      </c>
+      <c r="C584" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="585" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A585" t="s">
+        <v>6</v>
+      </c>
+      <c r="B585">
+        <v>44</v>
+      </c>
+      <c r="C585" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="586" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>6</v>
+      </c>
+      <c r="B586">
+        <v>45</v>
+      </c>
+      <c r="C586" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="587" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>6</v>
+      </c>
+      <c r="B587">
+        <v>46</v>
+      </c>
+      <c r="C587" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="588" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A588" t="s">
+        <v>6</v>
+      </c>
+      <c r="B588">
+        <v>47</v>
+      </c>
+      <c r="C588" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="589" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A589" t="s">
+        <v>6</v>
+      </c>
+      <c r="B589">
+        <v>48</v>
+      </c>
+      <c r="C589" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>6</v>
+      </c>
+      <c r="B590">
+        <v>49</v>
+      </c>
+      <c r="C590" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="591" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>6</v>
+      </c>
+      <c r="B591">
+        <v>50</v>
+      </c>
+      <c r="C591" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="592" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>6</v>
+      </c>
+      <c r="B592">
+        <v>51</v>
+      </c>
+      <c r="C592" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="593" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>6</v>
+      </c>
+      <c r="B593">
+        <v>52</v>
+      </c>
+      <c r="C593" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="594" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>6</v>
+      </c>
+      <c r="B594">
+        <v>53</v>
+      </c>
+      <c r="C594" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="595" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>6</v>
+      </c>
+      <c r="B595">
+        <v>54</v>
+      </c>
+      <c r="C595" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="596" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>6</v>
+      </c>
+      <c r="B596">
+        <v>55</v>
+      </c>
+      <c r="C596" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="597" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>6</v>
+      </c>
+      <c r="B597">
+        <v>56</v>
+      </c>
+      <c r="C597" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="598" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>6</v>
+      </c>
+      <c r="B598">
+        <v>57</v>
+      </c>
+      <c r="C598" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="599" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>6</v>
+      </c>
+      <c r="B599">
+        <v>58</v>
+      </c>
+      <c r="C599" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="600" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>6</v>
+      </c>
+      <c r="B600">
+        <v>59</v>
+      </c>
+      <c r="C600" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="601" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
+        <v>6</v>
+      </c>
+      <c r="B601">
+        <v>60</v>
+      </c>
+      <c r="C601" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="602" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
+        <v>6</v>
+      </c>
+      <c r="B602">
+        <v>61</v>
+      </c>
+      <c r="C602" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="603" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
+        <v>6</v>
+      </c>
+      <c r="B603">
+        <v>62</v>
+      </c>
+      <c r="C603" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
+        <v>6</v>
+      </c>
+      <c r="B604">
+        <v>63</v>
+      </c>
+      <c r="C604" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
+        <v>6</v>
+      </c>
+      <c r="B605">
+        <v>64</v>
+      </c>
+      <c r="C605" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="606" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A606" t="s">
+        <v>6</v>
+      </c>
+      <c r="B606">
+        <v>65</v>
+      </c>
+      <c r="C606" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A607" t="s">
+        <v>6</v>
+      </c>
+      <c r="B607">
+        <v>66</v>
+      </c>
+      <c r="C607" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="608" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A608" t="s">
+        <v>6</v>
+      </c>
+      <c r="B608">
+        <v>67</v>
+      </c>
+      <c r="C608" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="609" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>6</v>
+      </c>
+      <c r="B609">
+        <v>68</v>
+      </c>
+      <c r="C609" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="610" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A610" t="s">
+        <v>6</v>
+      </c>
+      <c r="B610">
+        <v>69</v>
+      </c>
+      <c r="C610" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
+        <v>6</v>
+      </c>
+      <c r="B611">
+        <v>70</v>
+      </c>
+      <c r="C611" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="612" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
+        <v>6</v>
+      </c>
+      <c r="B612">
+        <v>71</v>
+      </c>
+      <c r="C612" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
+        <v>6</v>
+      </c>
+      <c r="B613">
+        <v>72</v>
+      </c>
+      <c r="C613" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="614" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
+        <v>6</v>
+      </c>
+      <c r="B614">
+        <v>73</v>
+      </c>
+      <c r="C614" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="615" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
+        <v>6</v>
+      </c>
+      <c r="B615">
+        <v>74</v>
+      </c>
+      <c r="C615" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="616" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A616" t="s">
+        <v>6</v>
+      </c>
+      <c r="B616">
+        <v>75</v>
+      </c>
+      <c r="C616" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="617" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A617" t="s">
+        <v>6</v>
+      </c>
+      <c r="B617">
+        <v>76</v>
+      </c>
+      <c r="C617" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="618" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A618" t="s">
+        <v>6</v>
+      </c>
+      <c r="B618">
+        <v>77</v>
+      </c>
+      <c r="C618" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
+        <v>6</v>
+      </c>
+      <c r="B619">
+        <v>78</v>
+      </c>
+      <c r="C619" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
+        <v>6</v>
+      </c>
+      <c r="B620">
+        <v>79</v>
+      </c>
+      <c r="C620" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
+        <v>6</v>
+      </c>
+      <c r="B621">
+        <v>80</v>
+      </c>
+      <c r="C621" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
+        <v>6</v>
+      </c>
+      <c r="B622">
+        <v>81</v>
+      </c>
+      <c r="C622" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="623" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
+        <v>6</v>
+      </c>
+      <c r="B623">
+        <v>82</v>
+      </c>
+      <c r="C623" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="624" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A624" t="s">
+        <v>6</v>
+      </c>
+      <c r="B624">
+        <v>83</v>
+      </c>
+      <c r="C624" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A625" t="s">
+        <v>6</v>
+      </c>
+      <c r="B625">
+        <v>84</v>
+      </c>
+      <c r="C625" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="626" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A626" t="s">
+        <v>6</v>
+      </c>
+      <c r="B626">
+        <v>85</v>
+      </c>
+      <c r="C626" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="627" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A627" t="s">
+        <v>6</v>
+      </c>
+      <c r="B627">
+        <v>86</v>
+      </c>
+      <c r="C627" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="628" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
+        <v>6</v>
+      </c>
+      <c r="B628">
+        <v>87</v>
+      </c>
+      <c r="C628" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="629" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
+        <v>6</v>
+      </c>
+      <c r="B629">
+        <v>88</v>
+      </c>
+      <c r="C629" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="630" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
+        <v>6</v>
+      </c>
+      <c r="B630">
+        <v>89</v>
+      </c>
+      <c r="C630" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="631" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
+        <v>6</v>
+      </c>
+      <c r="B631">
+        <v>90</v>
+      </c>
+      <c r="C631" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="632" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
+        <v>6</v>
+      </c>
+      <c r="B632">
+        <v>91</v>
+      </c>
+      <c r="C632" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="633" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A633" t="s">
+        <v>6</v>
+      </c>
+      <c r="B633">
+        <v>92</v>
+      </c>
+      <c r="C633" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="634" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A634" t="s">
+        <v>6</v>
+      </c>
+      <c r="B634">
+        <v>93</v>
+      </c>
+      <c r="C634" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="635" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A635" t="s">
+        <v>6</v>
+      </c>
+      <c r="B635">
+        <v>94</v>
+      </c>
+      <c r="C635" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="636" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
+        <v>6</v>
+      </c>
+      <c r="B636">
+        <v>95</v>
+      </c>
+      <c r="C636" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A637" t="s">
+        <v>6</v>
+      </c>
+      <c r="B637">
+        <v>96</v>
+      </c>
+      <c r="C637" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A638" t="s">
+        <v>6</v>
+      </c>
+      <c r="B638">
+        <v>97</v>
+      </c>
+      <c r="C638" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="639" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
+        <v>6</v>
+      </c>
+      <c r="B639">
+        <v>98</v>
+      </c>
+      <c r="C639" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="640" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
+        <v>6</v>
+      </c>
+      <c r="B640">
+        <v>99</v>
+      </c>
+      <c r="C640" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
+        <v>6</v>
+      </c>
+      <c r="B641">
+        <v>100</v>
+      </c>
+      <c r="C641" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="642" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A642" t="s">
+        <v>6</v>
+      </c>
+      <c r="B642">
+        <v>101</v>
+      </c>
+      <c r="C642" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="643" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A643" t="s">
+        <v>6</v>
+      </c>
+      <c r="B643">
+        <v>102</v>
+      </c>
+      <c r="C643" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="644" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A644" t="s">
+        <v>6</v>
+      </c>
+      <c r="B644">
+        <v>103</v>
+      </c>
+      <c r="C644" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="645" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A645" t="s">
+        <v>6</v>
+      </c>
+      <c r="B645">
+        <v>104</v>
+      </c>
+      <c r="C645" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="646" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A646" t="s">
+        <v>6</v>
+      </c>
+      <c r="B646">
+        <v>105</v>
+      </c>
+      <c r="C646" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="647" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A647" t="s">
+        <v>6</v>
+      </c>
+      <c r="B647">
+        <v>106</v>
+      </c>
+      <c r="C647" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="648" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A648" t="s">
+        <v>6</v>
+      </c>
+      <c r="B648">
+        <v>107</v>
+      </c>
+      <c r="C648" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="649" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A649" t="s">
+        <v>6</v>
+      </c>
+      <c r="B649">
+        <v>108</v>
+      </c>
+      <c r="C649" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="650" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A650" t="s">
+        <v>6</v>
+      </c>
+      <c r="B650">
+        <v>109</v>
+      </c>
+      <c r="C650" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="651" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A651" t="s">
+        <v>6</v>
+      </c>
+      <c r="B651">
+        <v>110</v>
+      </c>
+      <c r="C651" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="652" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A652" t="s">
+        <v>6</v>
+      </c>
+      <c r="B652">
+        <v>111</v>
+      </c>
+      <c r="C652" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="653" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A653" t="s">
+        <v>6</v>
+      </c>
+      <c r="B653">
+        <v>112</v>
+      </c>
+      <c r="C653" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="654" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A654" t="s">
+        <v>6</v>
+      </c>
+      <c r="B654">
+        <v>113</v>
+      </c>
+      <c r="C654" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="655" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A655" t="s">
+        <v>6</v>
+      </c>
+      <c r="B655">
+        <v>114</v>
+      </c>
+      <c r="C655" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="656" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A656" t="s">
+        <v>6</v>
+      </c>
+      <c r="B656">
+        <v>115</v>
+      </c>
+      <c r="C656" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="657" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
+        <v>6</v>
+      </c>
+      <c r="B657">
+        <v>116</v>
+      </c>
+      <c r="C657" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="658" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A658" t="s">
+        <v>6</v>
+      </c>
+      <c r="B658">
+        <v>117</v>
+      </c>
+      <c r="C658" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="659" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A659" t="s">
+        <v>6</v>
+      </c>
+      <c r="B659">
+        <v>118</v>
+      </c>
+      <c r="C659" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="660" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A660" t="s">
+        <v>6</v>
+      </c>
+      <c r="B660">
+        <v>119</v>
+      </c>
+      <c r="C660" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="661" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A661" t="s">
+        <v>6</v>
+      </c>
+      <c r="B661">
+        <v>120</v>
+      </c>
+      <c r="C661" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="662" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A662" t="s">
+        <v>6</v>
+      </c>
+      <c r="B662">
+        <v>121</v>
+      </c>
+      <c r="C662" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="663" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A663" t="s">
+        <v>6</v>
+      </c>
+      <c r="B663">
+        <v>122</v>
+      </c>
+      <c r="C663" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="664" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A664" t="s">
+        <v>6</v>
+      </c>
+      <c r="B664">
+        <v>123</v>
+      </c>
+      <c r="C664" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="665" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A665" t="s">
+        <v>6</v>
+      </c>
+      <c r="B665">
+        <v>124</v>
+      </c>
+      <c r="C665" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="666" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A666" t="s">
+        <v>6</v>
+      </c>
+      <c r="B666">
+        <v>125</v>
+      </c>
+      <c r="C666" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="667" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A667" t="s">
+        <v>6</v>
+      </c>
+      <c r="B667">
+        <v>126</v>
+      </c>
+      <c r="C667" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="668" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A668" t="s">
+        <v>6</v>
+      </c>
+      <c r="B668">
+        <v>127</v>
+      </c>
+      <c r="C668" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="669" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A669" t="s">
+        <v>6</v>
+      </c>
+      <c r="B669">
+        <v>128</v>
+      </c>
+      <c r="C669" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="670" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A670" t="s">
+        <v>6</v>
+      </c>
+      <c r="B670">
+        <v>129</v>
+      </c>
+      <c r="C670" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="671" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A671" t="s">
+        <v>6</v>
+      </c>
+      <c r="B671">
+        <v>130</v>
+      </c>
+      <c r="C671" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="672" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A672" t="s">
+        <v>6</v>
+      </c>
+      <c r="B672">
+        <v>131</v>
+      </c>
+      <c r="C672" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="673" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A673" t="s">
+        <v>6</v>
+      </c>
+      <c r="B673">
+        <v>132</v>
+      </c>
+      <c r="C673" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="674" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A674" t="s">
+        <v>6</v>
+      </c>
+      <c r="B674">
+        <v>133</v>
+      </c>
+      <c r="C674" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="675" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A675" t="s">
+        <v>6</v>
+      </c>
+      <c r="B675">
+        <v>134</v>
+      </c>
+      <c r="C675" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="676" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A676" t="s">
+        <v>6</v>
+      </c>
+      <c r="B676">
+        <v>135</v>
+      </c>
+      <c r="C676" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="677" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A677" t="s">
+        <v>6</v>
+      </c>
+      <c r="B677">
+        <v>136</v>
+      </c>
+      <c r="C677" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="678" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A678" t="s">
+        <v>6</v>
+      </c>
+      <c r="B678">
+        <v>137</v>
+      </c>
+      <c r="C678" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="679" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A679" t="s">
+        <v>6</v>
+      </c>
+      <c r="B679">
+        <v>138</v>
+      </c>
+      <c r="C679" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="680" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A680" t="s">
+        <v>6</v>
+      </c>
+      <c r="B680">
+        <v>139</v>
+      </c>
+      <c r="C680" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="681" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A681" t="s">
+        <v>6</v>
+      </c>
+      <c r="B681">
+        <v>140</v>
+      </c>
+      <c r="C681" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="682" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A682" t="s">
+        <v>6</v>
+      </c>
+      <c r="B682">
+        <v>141</v>
+      </c>
+      <c r="C682" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="683" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A683" t="s">
+        <v>6</v>
+      </c>
+      <c r="B683">
+        <v>142</v>
+      </c>
+      <c r="C683" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="684" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A684" t="s">
+        <v>6</v>
+      </c>
+      <c r="B684">
+        <v>143</v>
+      </c>
+      <c r="C684" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="685" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A685" t="s">
+        <v>6</v>
+      </c>
+      <c r="B685">
+        <v>144</v>
+      </c>
+      <c r="C685" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="686" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A686" t="s">
+        <v>6</v>
+      </c>
+      <c r="B686">
+        <v>145</v>
+      </c>
+      <c r="C686" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="687" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A687" t="s">
+        <v>6</v>
+      </c>
+      <c r="B687">
+        <v>146</v>
+      </c>
+      <c r="C687" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="688" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A688" t="s">
+        <v>6</v>
+      </c>
+      <c r="B688">
+        <v>147</v>
+      </c>
+      <c r="C688" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="689" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A689" t="s">
+        <v>6</v>
+      </c>
+      <c r="B689">
+        <v>148</v>
+      </c>
+      <c r="C689" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="690" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A690" t="s">
+        <v>6</v>
+      </c>
+      <c r="B690">
+        <v>149</v>
+      </c>
+      <c r="C690" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="691" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A691" t="s">
+        <v>6</v>
+      </c>
+      <c r="B691">
+        <v>150</v>
+      </c>
+      <c r="C691" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="692" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A692" t="s">
+        <v>6</v>
+      </c>
+      <c r="B692">
+        <v>151</v>
+      </c>
+      <c r="C692" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="693" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A693" t="s">
+        <v>6</v>
+      </c>
+      <c r="B693">
+        <v>152</v>
+      </c>
+      <c r="C693" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="694" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
+        <v>6</v>
+      </c>
+      <c r="B694">
+        <v>153</v>
+      </c>
+      <c r="C694" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="695" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A695" t="s">
+        <v>6</v>
+      </c>
+      <c r="B695">
+        <v>154</v>
+      </c>
+      <c r="C695" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="696" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A696" t="s">
+        <v>6</v>
+      </c>
+      <c r="B696">
+        <v>155</v>
+      </c>
+      <c r="C696" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="697" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A697" t="s">
+        <v>6</v>
+      </c>
+      <c r="B697">
+        <v>156</v>
+      </c>
+      <c r="C697" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="698" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A698" t="s">
+        <v>6</v>
+      </c>
+      <c r="B698">
+        <v>157</v>
+      </c>
+      <c r="C698" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="699" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A699" t="s">
+        <v>6</v>
+      </c>
+      <c r="B699">
+        <v>158</v>
+      </c>
+      <c r="C699" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="700" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A700" t="s">
+        <v>6</v>
+      </c>
+      <c r="B700">
+        <v>159</v>
+      </c>
+      <c r="C700" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="701" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
+        <v>6</v>
+      </c>
+      <c r="B701">
+        <v>160</v>
+      </c>
+      <c r="C701" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="702" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A702" t="s">
+        <v>6</v>
+      </c>
+      <c r="B702">
+        <v>161</v>
+      </c>
+      <c r="C702" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="703" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A703" t="s">
+        <v>6</v>
+      </c>
+      <c r="B703">
+        <v>162</v>
+      </c>
+      <c r="C703" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="704" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A704" t="s">
+        <v>6</v>
+      </c>
+      <c r="B704">
+        <v>163</v>
+      </c>
+      <c r="C704" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="705" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A705" t="s">
+        <v>6</v>
+      </c>
+      <c r="B705">
+        <v>164</v>
+      </c>
+      <c r="C705" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="706" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A706" t="s">
+        <v>6</v>
+      </c>
+      <c r="B706">
+        <v>165</v>
+      </c>
+      <c r="C706" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="707" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A707" t="s">
+        <v>6</v>
+      </c>
+      <c r="B707">
+        <v>166</v>
+      </c>
+      <c r="C707" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="708" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A708" t="s">
+        <v>6</v>
+      </c>
+      <c r="B708">
+        <v>167</v>
+      </c>
+      <c r="C708" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="709" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A709" t="s">
+        <v>6</v>
+      </c>
+      <c r="B709">
+        <v>168</v>
+      </c>
+      <c r="C709" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="710" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A710" t="s">
+        <v>6</v>
+      </c>
+      <c r="B710">
+        <v>169</v>
+      </c>
+      <c r="C710" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="711" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A711" t="s">
+        <v>6</v>
+      </c>
+      <c r="B711">
+        <v>170</v>
+      </c>
+      <c r="C711" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="712" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A712" t="s">
+        <v>6</v>
+      </c>
+      <c r="B712">
+        <v>171</v>
+      </c>
+      <c r="C712" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="713" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A713" t="s">
+        <v>6</v>
+      </c>
+      <c r="B713">
+        <v>172</v>
+      </c>
+      <c r="C713" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="714" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A714" t="s">
+        <v>6</v>
+      </c>
+      <c r="B714">
+        <v>173</v>
+      </c>
+      <c r="C714" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="715" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A715" t="s">
+        <v>6</v>
+      </c>
+      <c r="B715">
+        <v>174</v>
+      </c>
+      <c r="C715" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="716" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A716" t="s">
+        <v>6</v>
+      </c>
+      <c r="B716">
+        <v>175</v>
+      </c>
+      <c r="C716" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="717" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A717" t="s">
+        <v>6</v>
+      </c>
+      <c r="B717">
+        <v>176</v>
+      </c>
+      <c r="C717" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="718" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A718" t="s">
+        <v>6</v>
+      </c>
+      <c r="B718">
+        <v>177</v>
+      </c>
+      <c r="C718" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="719" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A719" t="s">
+        <v>6</v>
+      </c>
+      <c r="B719">
+        <v>178</v>
+      </c>
+      <c r="C719" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="720" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A720" t="s">
+        <v>6</v>
+      </c>
+      <c r="B720">
+        <v>179</v>
+      </c>
+      <c r="C720" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="721" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A721" t="s">
+        <v>6</v>
+      </c>
+      <c r="B721">
+        <v>180</v>
+      </c>
+      <c r="C721" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>